<commit_message>
add detail pengeluaran report excel
</commit_message>
<xml_diff>
--- a/storage/template/Report_Template.xlsx
+++ b/storage/template/Report_Template.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\nursyifa-management\storage\template\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AB2D25-1506-435F-842C-53E003C63C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{92D2A038-B9F8-49BE-9C46-26DFC94D770E}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -42,7 +36,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -148,7 +142,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04750B3B-AC3C-418E-A0BA-FDEF7207E1A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{04750B3B-AC3C-418E-A0BA-FDEF7207E1A6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -220,7 +214,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -272,7 +266,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -466,36 +460,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC99AF11-7274-400C-8B35-B9A83F821CB8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="30.5546875" customWidth="1"/>
-    <col min="8" max="8" width="17.5546875" customWidth="1"/>
-    <col min="9" max="9" width="22.21875" customWidth="1"/>
-    <col min="10" max="11" width="16.44140625" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" customWidth="1"/>
+    <col min="10" max="11" width="16.42578125" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="6" t="s">
@@ -511,10 +505,10 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
-      <c r="N1" s="1"/>
+      <c r="N1" s="6"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
@@ -531,7 +525,7 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
@@ -548,7 +542,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="C1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>